<commit_message>
end of day (not a lot been done)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NapoleoneCyril.xlsx
+++ b/doc/Journal-de-Travail_NapoleoneCyril.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63blc\Documents\GitHub\P_App-183\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AA1A0B-B4B5-4A81-B8C5-5A323650E9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876A893F-8180-420B-B8B0-FC3171A3D343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -140,6 +140,18 @@
   </si>
   <si>
     <t>Prise en main de l'environment donné, utilisation du send et se faire une idée de ce qu'il y'a à faire</t>
+  </si>
+  <si>
+    <t>Reprise en main du projet car je me souvenais plus très bien où j'en étais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction erreur mysql et bcrypt au lancement de l'environment </t>
+  </si>
+  <si>
+    <t>Avancement projet, recherche sur OpenSSL et commencement implémentation</t>
+  </si>
+  <si>
+    <t>Désinstallation de bcrypt des modules et du code (adaptation) et installation de crypto(qui au final était en fait par défaut)</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1082,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0277777777777776E-2</c:v>
+                  <c:v>0.19791666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1088,7 +1100,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>3.8194444444444448E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,7 +2013,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2066,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 3 heurs 0 minutes</v>
+        <v>0 jours 6 heurs 0 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2069,15 +2081,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2161,11 +2173,13 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="str">
+      <c r="A9" s="16">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="50"/>
+        <v>13</v>
+      </c>
+      <c r="B9" s="50">
+        <v>45378</v>
+      </c>
       <c r="C9" s="51">
         <v>1</v>
       </c>
@@ -2219,15 +2233,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="str">
+      <c r="A11" s="16">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="50"/>
+        <v>16</v>
+      </c>
+      <c r="B11" s="50">
+        <v>45399</v>
+      </c>
       <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="52">
+        <v>25</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -2240,15 +2262,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="47"/>
+        <v>16</v>
+      </c>
+      <c r="B12" s="46">
+        <v>45399</v>
+      </c>
+      <c r="C12" s="47">
+        <v>1</v>
+      </c>
       <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2261,15 +2291,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+        <v>16</v>
+      </c>
+      <c r="B13" s="50">
+        <v>45399</v>
+      </c>
+      <c r="C13" s="51">
+        <v>1</v>
+      </c>
       <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="36"/>
+      <c r="E13" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2281,16 +2319,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+    <row r="14" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="46"/>
+        <v>16</v>
+      </c>
+      <c r="B14" s="46">
+        <v>45399</v>
+      </c>
       <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="48">
+        <v>35</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -8641,11 +8687,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8653,7 +8699,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>9.0277777777777776E-2</v>
+        <v>0.19791666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8753,7 +8799,7 @@
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -8761,7 +8807,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>3.8194444444444448E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -8770,7 +8816,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.12499999999999999</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9007,6 +9053,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9015,15 +9070,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9046,6 +9092,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9054,12 +9108,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
right routes + JDT update
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NapoleoneCyril.xlsx
+++ b/doc/Journal-de-Travail_NapoleoneCyril.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63blc\Documents\GitHub\P_App-183\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C21422-E768-4525-982A-B9BDBFDD705D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB02330C-D4CE-4256-A7B0-2CB0F8E993D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="3810" windowWidth="27660" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="555" yWindow="1350" windowWidth="27660" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Avancement (léger recommencement du projet), login fonctionnelle, signup fonctionnelle, recherche par nom exacte fonctionnelle, jwt pas encore implémenté ni OpenSSL</t>
+  </si>
+  <si>
+    <t>Amélioration des routes conformement au CDC</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1088,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30208333333333331</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2069,7 +2072,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 8 heurs 30 minutes</v>
+        <v>0 jours 9 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2088,11 +2091,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>150</v>
+        <v>195</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>510</v>
+        <v>555</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2383,15 +2386,23 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B16" s="46">
+        <v>45413</v>
+      </c>
       <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="48">
+        <v>45</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="55"/>
       <c r="O16">
         <v>40</v>
@@ -8704,7 +8715,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8712,7 +8723,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.30208333333333331</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8829,7 +8840,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.35416666666666663</v>
+        <v>0.38541666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9066,6 +9077,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9074,15 +9094,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9105,6 +9116,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9113,12 +9132,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
beginning of admin search (not working yet)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NapoleoneCyril.xlsx
+++ b/doc/Journal-de-Travail_NapoleoneCyril.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63blc\Documents\GitHub\P_App-183\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB02330C-D4CE-4256-A7B0-2CB0F8E993D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109A640D-79F2-47E4-A11A-DCE8088D31AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="1350" windowWidth="27660" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -158,6 +158,21 @@
   </si>
   <si>
     <t>Amélioration des routes conformement au CDC</t>
+  </si>
+  <si>
+    <t>Fonction de requête uniquement si le user est connecté au bon compte fonctionnel (apprentissage des variables de session)</t>
+  </si>
+  <si>
+    <t>Changement de port (j'ai eu un problème bête qui m'a fait perdre beaucoup de temps)</t>
+  </si>
+  <si>
+    <t>Commencement page admin avec recherche</t>
+  </si>
+  <si>
+    <t>Reinstallation de tout l'environment(github, code, docker, db, postman) car changement de classe</t>
+  </si>
+  <si>
+    <t>Fonction de recherche ADMIN (point 7.5) pas fini</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1103,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.60416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2019,7 +2034,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2087,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 15 minutes</v>
+        <v>0 jours 15 heurs 45 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2087,15 +2102,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>660</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>195</v>
+        <v>285</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>555</v>
+        <v>945</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2393,10 +2408,10 @@
       <c r="B16" s="46">
         <v>45413</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48">
-        <v>45</v>
-      </c>
+      <c r="C16" s="47">
+        <v>1</v>
+      </c>
+      <c r="D16" s="48"/>
       <c r="E16" s="49" t="s">
         <v>4</v>
       </c>
@@ -2408,73 +2423,119 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+    <row r="17" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B17" s="50">
+        <v>45413</v>
+      </c>
+      <c r="C17" s="51">
+        <v>1</v>
+      </c>
+      <c r="D17" s="52">
+        <v>30</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="56"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45420</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1</v>
+      </c>
+      <c r="D18" s="48">
+        <v>30</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45420</v>
+      </c>
+      <c r="C19" s="51">
+        <v>1</v>
+      </c>
       <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
+      <c r="E19" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" s="56"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="B20" s="46">
+        <v>45427</v>
+      </c>
       <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="36"/>
+      <c r="D20" s="48">
+        <v>45</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>42</v>
+      </c>
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
+      <c r="A21" s="16">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="36"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="50">
+        <v>45427</v>
+      </c>
+      <c r="C21" s="51">
+        <v>1</v>
+      </c>
+      <c r="D21" s="52">
+        <v>30</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>43</v>
+      </c>
       <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -8711,11 +8772,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>360</v>
+        <v>660</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>120</v>
+        <v>210</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8723,7 +8784,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.33333333333333331</v>
+        <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8840,7 +8901,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.38541666666666663</v>
+        <v>0.65624999999999989</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
beginning of openssl certification
reste plus qu'a faire le nécessaire dans server.js pour certifier + RAPPORT
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NapoleoneCyril.xlsx
+++ b/doc/Journal-de-Travail_NapoleoneCyril.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63blc\Documents\GitHub\P_App-183\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109A640D-79F2-47E4-A11A-DCE8088D31AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149C9053-F701-4047-AB4A-A0461FC4E7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Fonction de recherche ADMIN (point 7.5) pas fini</t>
+  </si>
+  <si>
+    <t>Fonction d'admins fonctionnels</t>
+  </si>
+  <si>
+    <t>Certification OPENSSL</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1109,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60416666666666663</c:v>
+                  <c:v>0.70833333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2034,7 +2040,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2087,7 +2093,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 15 heurs 45 minutes</v>
+        <v>0 jours 18 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2102,15 +2108,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>660</v>
+        <v>780</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>285</v>
+        <v>315</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>945</v>
+        <v>1095</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2539,27 +2545,45 @@
       <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="46">
+        <v>45434</v>
+      </c>
+      <c r="C22" s="47">
+        <v>1</v>
+      </c>
       <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="36"/>
+      <c r="E22" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="str">
+      <c r="A23" s="16">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="36"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="50">
+        <v>45434</v>
+      </c>
+      <c r="C23" s="51">
+        <v>1</v>
+      </c>
+      <c r="D23" s="52">
+        <v>30</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -8772,11 +8796,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>660</v>
+        <v>780</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8784,7 +8808,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.60416666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8901,7 +8925,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.65624999999999989</v>
+        <v>0.76041666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9138,15 +9162,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9155,6 +9170,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9177,14 +9201,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9193,4 +9209,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
db dump (and jdt)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_NapoleoneCyril.xlsx
+++ b/doc/Journal-de-Travail_NapoleoneCyril.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63blc\Documents\GitHub\P_App-183\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149C9053-F701-4047-AB4A-A0461FC4E7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B14D5C-2B76-4700-AE41-79BBFCBB99DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -178,7 +178,13 @@
     <t>Fonction d'admins fonctionnels</t>
   </si>
   <si>
-    <t>Certification OPENSSL</t>
+    <t>Certification OPENSSL (config)</t>
+  </si>
+  <si>
+    <t>Utilisation openssl fonctionnel (https ✔)</t>
+  </si>
+  <si>
+    <t>Présentations</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1115,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70833333333333337</c:v>
+                  <c:v>0.72916666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1121,7 +1127,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2040,7 +2046,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2099,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 18 heurs 15 minutes</v>
+        <v>0 jours 20 heurs 45 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2108,15 +2114,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>780</v>
+        <v>900</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>315</v>
+        <v>345</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>1095</v>
+        <v>1245</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2587,27 +2593,43 @@
       <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="46">
+        <v>45441</v>
+      </c>
       <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="36"/>
+      <c r="D24" s="48">
+        <v>30</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="G24" s="55"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="str">
+      <c r="A25" s="16">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="50">
+        <v>45440</v>
+      </c>
+      <c r="C25" s="51">
+        <v>2</v>
+      </c>
       <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="36"/>
+      <c r="E25" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="G25" s="56"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -8800,7 +8822,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8808,7 +8830,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.70833333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8868,7 +8890,7 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C9,'Journal de travail'!$D$7:$D$532)</f>
@@ -8880,7 +8902,7 @@
       </c>
       <c r="D9" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -8925,7 +8947,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.76041666666666663</v>
+        <v>0.86458333333333326</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9162,6 +9184,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9170,15 +9201,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9201,6 +9223,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9209,12 +9239,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>